<commit_message>
work plan has been partially filled in
</commit_message>
<xml_diff>
--- a/chart.xlsx
+++ b/chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="141" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="94" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Delovni list1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>1st year</t>
   </si>
@@ -50,16 +50,16 @@
     <t>WP1a</t>
   </si>
   <si>
-    <t>Imprecise probability trees</t>
-  </si>
-  <si>
-    <t>Joint models </t>
+    <t>Probability tree model</t>
+  </si>
+  <si>
+    <t>Joint models</t>
   </si>
   <si>
     <t>WP1b</t>
   </si>
   <si>
-    <t>Joint probability model</t>
+    <t>Expression for the joint</t>
   </si>
   <si>
     <t>basic properties</t>
@@ -68,7 +68,7 @@
     <t>WP1c</t>
   </si>
   <si>
-    <t>Lower and upper bounds</t>
+    <t>Mathematical properties</t>
   </si>
   <si>
     <t>B</t>
@@ -80,43 +80,43 @@
     <t>WP2a</t>
   </si>
   <si>
+    <t>Coefficients of ergodicity</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Computational</t>
+  </si>
+  <si>
+    <t>WP2b</t>
+  </si>
+  <si>
     <t>Computing bounds</t>
   </si>
   <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>Computational</t>
-  </si>
-  <si>
-    <t>WP2b</t>
+    <t>methods</t>
+  </si>
+  <si>
+    <t>WP2c</t>
   </si>
   <si>
     <t>Error estimation</t>
   </si>
   <si>
-    <t>methods</t>
-  </si>
-  <si>
-    <t>WP2c</t>
+    <t>WP2d</t>
   </si>
   <si>
     <t>Perturbation analysis</t>
   </si>
   <si>
-    <t>WP2d</t>
-  </si>
-  <si>
-    <t>Coefficients of ergodicity</t>
-  </si>
-  <si>
     <t>Research line 3</t>
   </si>
   <si>
     <t>WP3a</t>
   </si>
   <si>
-    <t>Conditions for convergence</t>
+    <t>Existence of limit distributions</t>
   </si>
   <si>
     <t>Limit behaviour</t>
@@ -131,7 +131,7 @@
     <t>WP3c</t>
   </si>
   <si>
-    <t>Classification of states</t>
+    <t>Characterise limit distriobutions</t>
   </si>
   <si>
     <t>Research line 4</t>
@@ -140,34 +140,19 @@
     <t>WP4a</t>
   </si>
   <si>
-    <t>Conceptual properties</t>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>WP4c</t>
+  </si>
+  <si>
+    <t>Research line 5</t>
+  </si>
+  <si>
+    <t>WP5a</t>
   </si>
   <si>
     <t>Time reversal</t>
-  </si>
-  <si>
-    <t>WP4b</t>
-  </si>
-  <si>
-    <t>Reversible chains</t>
-  </si>
-  <si>
-    <t>WP4c</t>
-  </si>
-  <si>
-    <t>Research line 5</t>
-  </si>
-  <si>
-    <t>WP5a</t>
-  </si>
-  <si>
-    <t>Applications</t>
-  </si>
-  <si>
-    <t>WP5b</t>
-  </si>
-  <si>
-    <t>WP5c</t>
   </si>
   <si>
     <t>G</t>
@@ -195,6 +180,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -216,6 +202,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -524,6 +511,14 @@
       <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="O4" s="0"/>
+      <c r="P4" s="0"/>
+      <c r="S4" s="0"/>
     </row>
     <row r="5" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
@@ -557,324 +552,345 @@
       <c r="P5" s="12"/>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+    <row r="6" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="12"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="12"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="12"/>
+      <c r="S6" s="13"/>
+    </row>
+    <row r="7" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="6"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="6"/>
-      <c r="S6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="D7" s="12"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="12"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="12"/>
+      <c r="S7" s="13"/>
+    </row>
+    <row r="8" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="6"/>
+      <c r="S8" s="7"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="L8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0"/>
-      <c r="B9" s="9" t="s">
+      <c r="D9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+      <c r="K9" s="0"/>
+      <c r="L9" s="0"/>
+      <c r="O9" s="0"/>
+      <c r="P9" s="0"/>
+      <c r="S9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="12"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="12"/>
-      <c r="S9" s="13"/>
-    </row>
-    <row r="10" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="D10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="0"/>
+      <c r="S10" s="0"/>
+    </row>
+    <row r="11" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="12"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="12"/>
+      <c r="S11" s="13"/>
+    </row>
+    <row r="12" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
-      <c r="J10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
-      <c r="S10" s="7"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="D12" s="6"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="6"/>
+      <c r="J12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O12" s="7"/>
+      <c r="P12" s="6"/>
+      <c r="S12" s="7"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B13" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="L11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11" t="s">
+      <c r="D13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="0"/>
+      <c r="S13" s="0"/>
+    </row>
+    <row r="14" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="12"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="12"/>
-      <c r="N12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="S12" s="13"/>
-    </row>
-    <row r="13" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="D14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="12"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="12"/>
+      <c r="N14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="S14" s="13"/>
+    </row>
+    <row r="15" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="J13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P13" s="6"/>
-      <c r="S13" s="7"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="D15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="6"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="R15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" s="10" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="D16" s="12"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="12"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="12"/>
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B17" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="P14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="R14" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" s="10" customFormat="true" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11" t="s">
+      <c r="C17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="12"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="12"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="12"/>
-      <c r="S15" s="13"/>
-    </row>
-    <row r="16" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="D17" s="6"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="6"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C18" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="6"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="6"/>
-      <c r="S16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" s="10" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="12"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="12"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="12"/>
-      <c r="S18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="0" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>